<commit_message>
Fix the issue with mailing
</commit_message>
<xml_diff>
--- a/data/recepients.xlsx
+++ b/data/recepients.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCF63DF-190A-4A38-8056-E086DEE7F90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,33 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email for Arm</t>
   </si>
   <si>
-    <t>vahan.hovhannisyan.h@gmail.com</t>
+    <t>gevorgadamyan@yahoo.com</t>
   </si>
   <si>
-    <t>eurotouram@yahoo.com</t>
+    <t>adamyangevorg4@gmail.com</t>
   </si>
   <si>
-    <t>eurotouram@gmail.com</t>
-  </si>
-  <si>
-    <t>lil-3@mail.ru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lilis88@mail.ru </t>
-  </si>
-  <si>
-    <t>levon.eurotour@gmail.com</t>
+    <t>gevorgadamyan@outlook.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,19 +410,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -445,43 +430,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{49124D8D-9335-4D84-8EE4-8524E1E6548C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{EF18C0F0-61E5-4A63-AA22-454073B5F048}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{ACE63076-80F0-4AAF-BC70-84F59F5B2E9D}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{DA11BA3A-5260-4287-95C5-FD28DAB4DAB4}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{04290EAA-803F-4E71-BEA6-FED3E5EDF8FA}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>